<commit_message>
HUGE commit. Made everything work finally.
</commit_message>
<xml_diff>
--- a/src/main/webapp/assets/workbook/PCs.xlsx
+++ b/src/main/webapp/assets/workbook/PCs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyler\Agile Programming\Excel speadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben.julian/IdeaProjects/Agile/2021_agile_tenebrae/src/main/webapp/assets/workbook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4796571-380F-4951-B640-85651C9BBDAC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBEC17E2-3CD5-2942-923D-DE524845C242}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CE545C04-5E23-4CB0-9461-E481141797D6}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{CE545C04-5E23-4CB0-9461-E481141797D6}"/>
   </bookViews>
   <sheets>
     <sheet name="PCs" sheetId="1" r:id="rId1"/>
@@ -34,55 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Class</t>
-  </si>
-  <si>
-    <t>Level</t>
-  </si>
-  <si>
-    <t>Race</t>
-  </si>
-  <si>
-    <t>Hit Points</t>
-  </si>
-  <si>
-    <t>Armor Class</t>
-  </si>
-  <si>
-    <t>Proficiency</t>
-  </si>
-  <si>
-    <t>Initiative</t>
-  </si>
-  <si>
-    <t>Speed</t>
-  </si>
-  <si>
-    <t>Strength</t>
-  </si>
-  <si>
-    <t>Dexterity</t>
-  </si>
-  <si>
-    <t>Constitution</t>
-  </si>
-  <si>
-    <t>Intelligence</t>
-  </si>
-  <si>
-    <t>Wisdom</t>
-  </si>
-  <si>
-    <t>Charisma</t>
-  </si>
-  <si>
-    <t>Background</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Benja Minn</t>
   </si>
@@ -108,32 +60,24 @@
     <t>Maat, a prodigy in arcana magic, grew up a lover of books and knowledge, admitting him into the High Council of Magic at the young age of 15.</t>
   </si>
   <si>
-    <t>Tie'l Urr</t>
-  </si>
-  <si>
     <t>Cleric</t>
   </si>
   <si>
     <t>Dwarf</t>
   </si>
   <si>
-    <t>The cleric Tie'l taught the ways of his holy god to his fellow Dwarves in the great mountain of Stormwind Peak.</t>
+    <t>Tie''l Urr</t>
+  </si>
+  <si>
+    <t>The cleric Tie''l taught the ways of his holy god to his fellow Dwarves in the great mountain of Stormwind Peak.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -161,9 +105,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -478,93 +421,93 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D8C2DCA-0740-4737-94FB-877AB7E3E0C9}">
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="129.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="129.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1">
+        <v>48</v>
+      </c>
+      <c r="F1">
+        <v>15</v>
+      </c>
+      <c r="G1">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1">
+        <v>2</v>
+      </c>
+      <c r="I1">
+        <v>30</v>
+      </c>
+      <c r="J1">
+        <v>10</v>
+      </c>
+      <c r="K1">
+        <v>13</v>
+      </c>
+      <c r="L1">
+        <v>18</v>
+      </c>
+      <c r="M1">
+        <v>11</v>
+      </c>
+      <c r="N1">
+        <v>18</v>
+      </c>
+      <c r="O1">
+        <v>9</v>
+      </c>
+      <c r="P1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="B2" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" t="s">
-        <v>17</v>
       </c>
       <c r="C2">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="E2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="F2">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G2">
         <v>3</v>
@@ -576,125 +519,75 @@
         <v>30</v>
       </c>
       <c r="J2">
+        <v>8</v>
+      </c>
+      <c r="K2">
+        <v>14</v>
+      </c>
+      <c r="L2">
+        <v>13</v>
+      </c>
+      <c r="M2">
+        <v>17</v>
+      </c>
+      <c r="N2">
+        <v>7</v>
+      </c>
+      <c r="O2">
+        <v>15</v>
+      </c>
+      <c r="P2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="K2">
-        <v>13</v>
-      </c>
-      <c r="L2">
-        <v>18</v>
-      </c>
-      <c r="M2">
-        <v>11</v>
-      </c>
-      <c r="N2">
-        <v>18</v>
-      </c>
-      <c r="O2">
-        <v>9</v>
-      </c>
-      <c r="P2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="E3">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="F3">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G3">
         <v>3</v>
       </c>
       <c r="H3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I3">
         <v>30</v>
       </c>
       <c r="J3">
+        <v>10</v>
+      </c>
+      <c r="K3">
+        <v>12</v>
+      </c>
+      <c r="L3">
+        <v>15</v>
+      </c>
+      <c r="M3">
         <v>8</v>
       </c>
-      <c r="K3">
-        <v>14</v>
-      </c>
-      <c r="L3">
-        <v>13</v>
-      </c>
-      <c r="M3">
+      <c r="N3">
         <v>17</v>
       </c>
-      <c r="N3">
-        <v>7</v>
-      </c>
       <c r="O3">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="P3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4">
-        <v>46</v>
-      </c>
-      <c r="F4">
-        <v>17</v>
-      </c>
-      <c r="G4">
-        <v>3</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>30</v>
-      </c>
-      <c r="J4">
-        <v>10</v>
-      </c>
-      <c r="K4">
-        <v>12</v>
-      </c>
-      <c r="L4">
-        <v>15</v>
-      </c>
-      <c r="M4">
-        <v>8</v>
-      </c>
-      <c r="N4">
-        <v>17</v>
-      </c>
-      <c r="O4">
-        <v>9</v>
-      </c>
-      <c r="P4" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>